<commit_message>
this added by last report 15-05-25
</commit_message>
<xml_diff>
--- a/DD-Profit_ROI/Mangrove April-25 Profit and Loss.xlsx
+++ b/DD-Profit_ROI/Mangrove April-25 Profit and Loss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mangrove\DD-Profit_ROI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290DBE4A-6B9E-4034-8B92-E3E0138FC04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83991882-74AA-44C4-9F79-284F5B7FDD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,9 +1404,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="16"/>
-      <c r="C15" s="16">
-        <v>8100</v>
-      </c>
+      <c r="C15" s="16"/>
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
     </row>
@@ -1432,7 +1430,7 @@
       </c>
       <c r="C17" s="21">
         <f>SUM(C11:C16)</f>
-        <v>43624.31</v>
+        <v>35524.31</v>
       </c>
       <c r="G17" s="19"/>
     </row>
@@ -1752,7 +1750,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="62">
         <f>C17-F41</f>
-        <v>-33334.69</v>
+        <v>-41434.69</v>
       </c>
       <c r="G43" s="63"/>
     </row>

</xml_diff>